<commit_message>
corrected multiple worksheets articles
</commit_message>
<xml_diff>
--- a/source/_static/files/document-generation/demos/multiple-worksheets-template.xlsx
+++ b/source/_static/files/document-generation/demos/multiple-worksheets-template.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Templater\TemplaterTest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stoun\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DF39EF0-FF79-4589-B19D-FEE4DC97A289}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA1F7B23-FDCB-42AD-B3D9-2CFD30F6B33E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{EBBF3CE7-00CC-40E9-A5CA-46E9AA15742B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{EBBF3CE7-00CC-40E9-A5CA-46E9AA15742B}"/>
   </bookViews>
   <sheets>
-    <sheet name="{{name}}" sheetId="1" r:id="rId1"/>
+    <sheet name="{{sheetName}}" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -228,7 +228,7 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DFDB7636-02C1-4455-88E1-FF8753F10953}" name="Table1" displayName="Table1" ref="A3:B6" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{A31FE441-7ECD-41AC-9B4D-A6F3A11BFCC2}" name="Column1" headerRowDxfId="0" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{A31FE441-7ECD-41AC-9B4D-A6F3A11BFCC2}" name="Column1" headerRowDxfId="1" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{696715D1-510F-4373-AFBC-DB05B52255C9}" name="Column2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -555,7 +555,7 @@
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>